<commit_message>
Write Test Result to Excel File in Automation
</commit_message>
<xml_diff>
--- a/doc/cubecart-login.xlsx
+++ b/doc/cubecart-login.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unitedcoder\IdeaProjects\cubecartusa2021\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C93FF25-3F86-41AD-A94F-3688F3D07137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C74AE1-902C-408E-BD05-9768B322900B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,12 +87,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -108,13 +114,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -336,8 +343,8 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -354,7 +361,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -373,7 +380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ABFD66F-D5DD-4AC2-8A11-334349F935C4}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>